<commit_message>
commit: completed M.A.D.S | debug conversion to .exe file
</commit_message>
<xml_diff>
--- a/df_blk_output.xlsx
+++ b/df_blk_output.xlsx
@@ -2861,7 +2861,7 @@
     <t>Processing_Date</t>
   </si>
   <si>
-    <t>2025-08-29 14:34:13</t>
+    <t>2025-09-02 16:52:01</t>
   </si>
 </sst>
 </file>
@@ -3269,7 +3269,7 @@
         <v>9</v>
       </c>
       <c r="C2">
-        <v>251300005</v>
+        <v>251100004</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
@@ -3298,7 +3298,7 @@
         <v>9</v>
       </c>
       <c r="C3">
-        <v>251300005</v>
+        <v>251100004</v>
       </c>
       <c r="D3" t="s">
         <v>11</v>
@@ -3327,7 +3327,7 @@
         <v>9</v>
       </c>
       <c r="C4">
-        <v>251300005</v>
+        <v>251100004</v>
       </c>
       <c r="D4" t="s">
         <v>12</v>
@@ -3356,7 +3356,7 @@
         <v>9</v>
       </c>
       <c r="C5">
-        <v>251300005</v>
+        <v>251100004</v>
       </c>
       <c r="D5" t="s">
         <v>13</v>
@@ -3385,7 +3385,7 @@
         <v>9</v>
       </c>
       <c r="C6">
-        <v>251300005</v>
+        <v>251100004</v>
       </c>
       <c r="D6" t="s">
         <v>14</v>
@@ -3414,7 +3414,7 @@
         <v>9</v>
       </c>
       <c r="C7">
-        <v>251300005</v>
+        <v>251100004</v>
       </c>
       <c r="D7" t="s">
         <v>15</v>
@@ -3443,7 +3443,7 @@
         <v>9</v>
       </c>
       <c r="C8">
-        <v>251300005</v>
+        <v>251100004</v>
       </c>
       <c r="D8" t="s">
         <v>16</v>
@@ -3472,7 +3472,7 @@
         <v>9</v>
       </c>
       <c r="C9">
-        <v>251300005</v>
+        <v>251100004</v>
       </c>
       <c r="D9" t="s">
         <v>17</v>
@@ -3501,7 +3501,7 @@
         <v>9</v>
       </c>
       <c r="C10">
-        <v>251300005</v>
+        <v>251100004</v>
       </c>
       <c r="D10" t="s">
         <v>18</v>
@@ -3530,7 +3530,7 @@
         <v>9</v>
       </c>
       <c r="C11">
-        <v>251300005</v>
+        <v>251100004</v>
       </c>
       <c r="D11" t="s">
         <v>19</v>
@@ -3559,7 +3559,7 @@
         <v>9</v>
       </c>
       <c r="C12">
-        <v>251300005</v>
+        <v>251100004</v>
       </c>
       <c r="D12" t="s">
         <v>20</v>
@@ -3588,7 +3588,7 @@
         <v>9</v>
       </c>
       <c r="C13">
-        <v>251300005</v>
+        <v>251100004</v>
       </c>
       <c r="D13" t="s">
         <v>21</v>
@@ -3617,7 +3617,7 @@
         <v>9</v>
       </c>
       <c r="C14">
-        <v>251300005</v>
+        <v>251100004</v>
       </c>
       <c r="D14" t="s">
         <v>22</v>
@@ -3646,7 +3646,7 @@
         <v>9</v>
       </c>
       <c r="C15">
-        <v>251300005</v>
+        <v>251100004</v>
       </c>
       <c r="D15" t="s">
         <v>23</v>
@@ -3675,7 +3675,7 @@
         <v>9</v>
       </c>
       <c r="C16">
-        <v>251300005</v>
+        <v>251100004</v>
       </c>
       <c r="D16" t="s">
         <v>24</v>
@@ -3704,7 +3704,7 @@
         <v>9</v>
       </c>
       <c r="C17">
-        <v>251300005</v>
+        <v>251100004</v>
       </c>
       <c r="D17" t="s">
         <v>25</v>
@@ -3733,7 +3733,7 @@
         <v>9</v>
       </c>
       <c r="C18">
-        <v>251300005</v>
+        <v>251100004</v>
       </c>
       <c r="D18" t="s">
         <v>26</v>
@@ -3762,7 +3762,7 @@
         <v>9</v>
       </c>
       <c r="C19">
-        <v>251300005</v>
+        <v>251100004</v>
       </c>
       <c r="D19" t="s">
         <v>27</v>
@@ -70982,7 +70982,7 @@
         <v>9</v>
       </c>
       <c r="C2">
-        <v>251300005</v>
+        <v>251100004</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
@@ -71011,7 +71011,7 @@
         <v>9</v>
       </c>
       <c r="C3">
-        <v>251300005</v>
+        <v>251100004</v>
       </c>
       <c r="D3" t="s">
         <v>11</v>
@@ -71040,7 +71040,7 @@
         <v>9</v>
       </c>
       <c r="C4">
-        <v>251300005</v>
+        <v>251100004</v>
       </c>
       <c r="D4" t="s">
         <v>12</v>
@@ -71069,7 +71069,7 @@
         <v>9</v>
       </c>
       <c r="C5">
-        <v>251300005</v>
+        <v>251100004</v>
       </c>
       <c r="D5" t="s">
         <v>13</v>
@@ -71098,7 +71098,7 @@
         <v>9</v>
       </c>
       <c r="C6">
-        <v>251300005</v>
+        <v>251100004</v>
       </c>
       <c r="D6" t="s">
         <v>14</v>
@@ -71127,7 +71127,7 @@
         <v>9</v>
       </c>
       <c r="C7">
-        <v>251300005</v>
+        <v>251100004</v>
       </c>
       <c r="D7" t="s">
         <v>15</v>
@@ -71156,7 +71156,7 @@
         <v>9</v>
       </c>
       <c r="C8">
-        <v>251300005</v>
+        <v>251100004</v>
       </c>
       <c r="D8" t="s">
         <v>16</v>
@@ -71185,7 +71185,7 @@
         <v>9</v>
       </c>
       <c r="C9">
-        <v>251300005</v>
+        <v>251100004</v>
       </c>
       <c r="D9" t="s">
         <v>17</v>
@@ -71214,7 +71214,7 @@
         <v>9</v>
       </c>
       <c r="C10">
-        <v>251300005</v>
+        <v>251100004</v>
       </c>
       <c r="D10" t="s">
         <v>18</v>
@@ -71243,7 +71243,7 @@
         <v>9</v>
       </c>
       <c r="C11">
-        <v>251300005</v>
+        <v>251100004</v>
       </c>
       <c r="D11" t="s">
         <v>19</v>
@@ -71272,7 +71272,7 @@
         <v>9</v>
       </c>
       <c r="C12">
-        <v>251300005</v>
+        <v>251100004</v>
       </c>
       <c r="D12" t="s">
         <v>20</v>
@@ -71301,7 +71301,7 @@
         <v>9</v>
       </c>
       <c r="C13">
-        <v>251300005</v>
+        <v>251100004</v>
       </c>
       <c r="D13" t="s">
         <v>21</v>
@@ -71330,7 +71330,7 @@
         <v>9</v>
       </c>
       <c r="C14">
-        <v>251300005</v>
+        <v>251100004</v>
       </c>
       <c r="D14" t="s">
         <v>22</v>
@@ -71359,7 +71359,7 @@
         <v>9</v>
       </c>
       <c r="C15">
-        <v>251300005</v>
+        <v>251100004</v>
       </c>
       <c r="D15" t="s">
         <v>23</v>
@@ -71388,7 +71388,7 @@
         <v>9</v>
       </c>
       <c r="C16">
-        <v>251300005</v>
+        <v>251100004</v>
       </c>
       <c r="D16" t="s">
         <v>24</v>
@@ -71417,7 +71417,7 @@
         <v>9</v>
       </c>
       <c r="C17">
-        <v>251300005</v>
+        <v>251100004</v>
       </c>
       <c r="D17" t="s">
         <v>25</v>
@@ -71446,7 +71446,7 @@
         <v>9</v>
       </c>
       <c r="C18">
-        <v>251300005</v>
+        <v>251100004</v>
       </c>
       <c r="D18" t="s">
         <v>26</v>
@@ -71475,7 +71475,7 @@
         <v>9</v>
       </c>
       <c r="C19">
-        <v>251300005</v>
+        <v>251100004</v>
       </c>
       <c r="D19" t="s">
         <v>27</v>
@@ -71528,7 +71528,7 @@
         <v>283</v>
       </c>
       <c r="B2">
-        <v>251300005</v>
+        <v>251100004</v>
       </c>
       <c r="C2">
         <v>18</v>

</xml_diff>